<commit_message>
Implement Handsontable for business.
</commit_message>
<xml_diff>
--- a/inventory/staticfiles/template_file/template.xlsx
+++ b/inventory/staticfiles/template_file/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pythonProjects\Inventory\inventory\staticfiles\template_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EED5F4F-8C64-4A57-B010-1A6D5BA65438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DA0E00-EDFE-4EE0-A360-23F9ADD1FC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12930" yWindow="1935" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="2340" windowWidth="25995" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>device_name</t>
   </si>
@@ -94,12 +94,6 @@
   </si>
   <si>
     <t>operating_system</t>
-  </si>
-  <si>
-    <t>supplier</t>
-  </si>
-  <si>
-    <t>business</t>
   </si>
 </sst>
 </file>
@@ -457,7 +451,7 @@
   <dimension ref="A2:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,12 +529,8 @@
       <c r="W2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made some CSS. Fix upload view for devices.
</commit_message>
<xml_diff>
--- a/inventory/staticfiles/template_file/template.xlsx
+++ b/inventory/staticfiles/template_file/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pythonProjects\Inventory\inventory\staticfiles\template_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DA0E00-EDFE-4EE0-A360-23F9ADD1FC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA241192-CEFD-4219-AEDF-45EF9A857D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="2340" windowWidth="25995" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>device_name</t>
   </si>
@@ -94,6 +94,74 @@
   </si>
   <si>
     <t>operating_system</t>
+  </si>
+  <si>
+    <t>Hostname
+[required,
+unique]</t>
+  </si>
+  <si>
+    <t>[not reqired]</t>
+  </si>
+  <si>
+    <t>[In operation,
+Decommissioned,
+Pending Setup,
+Offline,
+Not defined yet,
+Exception]</t>
+  </si>
+  <si>
+    <t>[Network,
+Server - Virtual,
+Server - Physical,
+ Server - Platform,
+Printer/Scanner, 
+Storage, 
+Conferencing, 
+End Users Computing, 
+AirCon, 
+UPS, 
+Other]</t>
+  </si>
+  <si>
+    <t>[Router,
+Firewall,
+Firewall/IDS/IPS,
+Access Point,
+Switch,
+Desktop,
+Laptop,
+Printer/MFP,
+Scanner,
+IP Phone,
+Teleconferencing/Modem,
+VoIP System - Cisco CM,
+VoIP System - other,
+App and DB Server,
+Application Server,
+Database Server,
+File Server,
+Other Server,
+Backup device,
+Storage - NAS,
+Storage - SAN,
+Data Historian,
+Human Machine Interface (HMI),
+IDS/IPS Detection,
+Master Terminal Unit (MTU),
+Programmable Logic Controller (PLC),
+Remote Access,
+Remote Terminal Unit (RTU),
+Other hardware]</t>
+  </si>
+  <si>
+    <t>default=1
+[not reqired]</t>
+  </si>
+  <si>
+    <t>default=today
+[not reqired]</t>
   </si>
 </sst>
 </file>
@@ -160,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -168,6 +236,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,17 +519,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Y2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>

</xml_diff>